<commit_message>
Add case for clpi
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_clpi.xlsx
+++ b/andes/cases/ieee14/ieee14_clpi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571A02B9-B7F8-E045-A53B-6CE5C286F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5883937-57D2-1C48-9AF8-9AA7F1AE65CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="-2520" windowWidth="34560" windowHeight="19440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="-3600" windowWidth="19200" windowHeight="21600" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1082,7 @@
         <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>